<commit_message>
complete the implementation of UI
</commit_message>
<xml_diff>
--- a/Project/results_extra_rgrowing_glcm.xlsx
+++ b/Project/results_extra_rgrowing_glcm.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="1713">
   <si>
     <t>final_1</t>
   </si>
@@ -2392,6 +2392,1110 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>final_1</t>
+  </si>
+  <si>
+    <t>final_2</t>
+  </si>
+  <si>
+    <t>final_3</t>
+  </si>
+  <si>
+    <t>final_4</t>
+  </si>
+  <si>
+    <t>final_5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>Contrast</t>
@@ -4068,7 +5172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -4086,11 +5190,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -4102,6 +5208,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4123,19 +5231,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1161</v>
+        <v>1529</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1162</v>
+        <v>1530</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1163</v>
+        <v>1531</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1164</v>
+        <v>1532</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1165</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="2">
@@ -4152,7 +5260,7 @@
         <v>0.99926518997562408</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1166</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="3">
@@ -4169,7 +5277,7 @@
         <v>0.99909223729108332</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1167</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="4">
@@ -4186,7 +5294,7 @@
         <v>0.99881704185932729</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1167</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="5">
@@ -4203,7 +5311,7 @@
         <v>0.99843864814066308</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1168</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="6">
@@ -4218,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1168</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="7">
@@ -4233,7 +5341,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1169</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="8">
@@ -4250,7 +5358,7 @@
         <v>0.99895081741643077</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1169</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="9">
@@ -4267,7 +5375,7 @@
         <v>0.99963880599582033</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1169</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="10">
@@ -4282,7 +5390,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1169</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="11">
@@ -4299,7 +5407,7 @@
         <v>0.99918779126044288</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1170</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="12">
@@ -4314,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1171</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="13">
@@ -4329,7 +5437,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1172</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="14">
@@ -4346,7 +5454,7 @@
         <v>0.99900050548049779</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1172</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="15">
@@ -4363,7 +5471,7 @@
         <v>0.99887437424094316</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1173</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="16">
@@ -4380,7 +5488,7 @@
         <v>0.99875970947771142</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>1174</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="17">
@@ -4397,7 +5505,7 @@
         <v>0.99925945673746264</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>1175</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="18">
@@ -4414,7 +5522,7 @@
         <v>0.99914956967269886</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>1176</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="19">
@@ -4431,7 +5539,7 @@
         <v>0.99934832192896694</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1177</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="20">
@@ -4448,7 +5556,7 @@
         <v>0.99845775893453514</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>1178</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="21">
@@ -4465,7 +5573,7 @@
         <v>0.99843673706127589</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>1179</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="22">
@@ -4482,7 +5590,7 @@
         <v>0.99897566144846439</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>1180</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="23">
@@ -4499,7 +5607,7 @@
         <v>0.99932061127785288</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1181</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="24">
@@ -4516,7 +5624,7 @@
         <v>0.99892024014623582</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>1182</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="25">
@@ -4533,7 +5641,7 @@
         <v>0.99908554851322806</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>1183</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="26">
@@ -4550,7 +5658,7 @@
         <v>0.99979455896587666</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1184</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="27">
@@ -4565,7 +5673,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1185</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="28">
@@ -4580,7 +5688,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1185</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="29">
@@ -4597,7 +5705,7 @@
         <v>0.99983755825208853</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>1186</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="30">
@@ -4614,7 +5722,7 @@
         <v>0.99883710819289295</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>1187</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="31">
@@ -4631,7 +5739,7 @@
         <v>0.99895272849581795</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>1188</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="32">
@@ -4648,7 +5756,7 @@
         <v>0.99885621898676469</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>1189</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="33">
@@ -4665,7 +5773,7 @@
         <v>0.99890208489205734</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>1190</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="34">
@@ -4682,7 +5790,7 @@
         <v>0.99908554851322806</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="35">
@@ -4699,7 +5807,7 @@
         <v>0.99899763886141724</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="36">
@@ -4716,7 +5824,7 @@
         <v>0.99950120827994249</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="37">
@@ -4733,7 +5841,7 @@
         <v>0.99958720685236613</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="38">
@@ -4750,7 +5858,7 @@
         <v>0.99944865359679469</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="39">
@@ -4767,7 +5875,7 @@
         <v>0.99946871993036024</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="40">
@@ -4784,7 +5892,7 @@
         <v>0.99937794365946864</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="41">
@@ -4801,7 +5909,7 @@
         <v>0.99941712078690614</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="42">
@@ -4818,7 +5926,7 @@
         <v>0.99946680885097305</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="43">
@@ -4835,7 +5943,7 @@
         <v>0.9995814736142048</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="44">
@@ -4852,7 +5960,7 @@
         <v>0.99951363029595941</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="45">
@@ -4869,7 +5977,7 @@
         <v>0.99941329862813166</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="46">
@@ -4886,7 +5994,7 @@
         <v>0.99944483143802021</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="47">
@@ -4901,7 +6009,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="48">
@@ -4916,7 +6024,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="49">
@@ -4931,7 +6039,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="50">
@@ -4948,7 +6056,7 @@
         <v>0.99820549645542567</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="51">
@@ -4965,7 +6073,7 @@
         <v>0.99851509131615068</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="52">
@@ -4982,7 +6090,7 @@
         <v>0.9993177446587721</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="53">
@@ -4999,7 +6107,7 @@
         <v>0.99942189848537411</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="54">
@@ -5016,7 +6124,7 @@
         <v>0.99863644485723757</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="55">
@@ -5033,7 +6141,7 @@
         <v>0.99901531634574858</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="56">
@@ -5050,7 +6158,7 @@
         <v>0.99912472564066546</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="57">
@@ -5067,7 +6175,7 @@
         <v>0.99921359083216987</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="58">
@@ -5084,7 +6192,7 @@
         <v>0.99903968260793552</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>1191</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="59">
@@ -5101,7 +6209,7 @@
         <v>0.99929481170612566</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>1192</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="60">
@@ -5116,7 +6224,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>1193</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="61">
@@ -5131,7 +6239,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>1194</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="62">
@@ -5148,7 +6256,7 @@
         <v>0.99912472564066546</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>1194</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="63">
@@ -5165,7 +6273,7 @@
         <v>0.99898091691677915</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>1194</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="64">
@@ -5182,7 +6290,7 @@
         <v>0.99926232335654341</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>1195</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="65">
@@ -5199,7 +6307,7 @@
         <v>0.99917728032381337</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>1196</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="66">
@@ -5216,7 +6324,7 @@
         <v>0.99904350476670989</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>1196</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="67">
@@ -5231,7 +6339,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>1196</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="68">
@@ -5248,7 +6356,7 @@
         <v>0.99827620639275161</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>1196</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="69">
@@ -5265,7 +6373,7 @@
         <v>0.99863166715876961</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>1196</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="70">
@@ -5280,7 +6388,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>1197</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="71">
@@ -5295,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>1198</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="72">
@@ -5312,7 +6420,7 @@
         <v>0.99911994794219749</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>1198</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="73">
@@ -5329,7 +6437,7 @@
         <v>0.99906357110027522</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>1199</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="74">
@@ -5346,7 +6454,7 @@
         <v>0.9994228540250677</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>1200</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="75">
@@ -5363,7 +6471,7 @@
         <v>0.99929863386489992</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>1200</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="76">
@@ -5378,7 +6486,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>1201</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="77">
@@ -5395,7 +6503,7 @@
         <v>0.99967607204387077</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>1202</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="78">
@@ -5410,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>1202</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="79">
@@ -5425,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>1202</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="80">
@@ -5442,7 +6550,7 @@
         <v>0.9993301666747888</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>1202</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="81">
@@ -5457,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>1203</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="82">
@@ -5474,7 +6582,7 @@
         <v>0.99914670305361808</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>1203</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="83">
@@ -5491,7 +6599,7 @@
         <v>0.99948878626392568</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>1204</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="84">
@@ -5508,7 +6616,7 @@
         <v>0.99903203829038667</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>1205</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="85">
@@ -5525,7 +6633,7 @@
         <v>0.99886195222492624</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="86">
@@ -5542,7 +6650,7 @@
         <v>0.99927092321378574</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="87">
@@ -5559,7 +6667,7 @@
         <v>0.99967607204387077</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="88">
@@ -5574,7 +6682,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="89">
@@ -5589,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="90">
@@ -5606,7 +6714,7 @@
         <v>0.99938845459609826</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>1206</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="91">
@@ -5623,7 +6731,7 @@
         <v>0.99900337209957857</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>1207</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="92">
@@ -5638,7 +6746,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>1208</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="93">
@@ -5653,7 +6761,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>1209</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="94">
@@ -5670,7 +6778,7 @@
         <v>0.99911517024372942</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>1210</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="95">
@@ -5685,7 +6793,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>1210</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="96">
@@ -5702,7 +6810,7 @@
         <v>0.99914096981545675</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>1211</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="97">
@@ -5719,7 +6827,7 @@
         <v>0.99911612578342313</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>1212</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="98">
@@ -5736,7 +6844,7 @@
         <v>0.99879506444637478</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>1213</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="99">
@@ -5751,7 +6859,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>1214</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="100">
@@ -5768,7 +6876,7 @@
         <v>0.99932443343662714</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>1215</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="101">
@@ -5785,7 +6893,7 @@
         <v>0.99891928460654222</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>1216</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="102">
@@ -5802,7 +6910,7 @@
         <v>0.99935309962743502</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>1216</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="103">
@@ -5819,7 +6927,7 @@
         <v>0.99926614551531778</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>1217</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="104">
@@ -5836,7 +6944,7 @@
         <v>0.99942763172353566</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>1218</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="105">
@@ -5853,7 +6961,7 @@
         <v>0.99940565431058281</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>1219</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="106">
@@ -5870,7 +6978,7 @@
         <v>0.99828193963091327</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>1220</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="107">
@@ -5887,7 +6995,7 @@
         <v>0.99888679625695997</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>1221</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="108">
@@ -5904,7 +7012,7 @@
         <v>0.998214096312668</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>1222</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="109">
@@ -5921,7 +7029,7 @@
         <v>0.99833544985375455</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>1223</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="110">
@@ -5938,7 +7046,7 @@
         <v>0.99912950333913342</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>1223</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="111">
@@ -5955,7 +7063,7 @@
         <v>0.99923652378481642</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>1224</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="112">
@@ -5972,7 +7080,7 @@
         <v>0.99893170662255903</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>1224</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="113">
@@ -5989,7 +7097,7 @@
         <v>0.99882181955779525</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>1225</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="114">
@@ -6006,7 +7114,7 @@
         <v>0.99940469877088933</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>1225</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="115">
@@ -6023,7 +7131,7 @@
         <v>0.99950980813718493</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>1225</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="116">
@@ -6040,7 +7148,7 @@
         <v>0.99862880053968883</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>1226</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="117">
@@ -6057,7 +7165,7 @@
         <v>0.99919448003829792</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>1227</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="118">
@@ -6074,7 +7182,7 @@
         <v>0.9992909895473514</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>1228</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="119">
@@ -6091,7 +7199,7 @@
         <v>0.99901388303620819</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>1229</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="120">
@@ -6108,7 +7216,7 @@
         <v>0.99932156681754647</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>1229</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="121">
@@ -6125,7 +7233,7 @@
         <v>0.99948209748607075</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>1230</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="122">
@@ -6142,7 +7250,7 @@
         <v>0.99910179268801902</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>1231</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="123">
@@ -6159,7 +7267,7 @@
         <v>0.99920690205431473</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>1232</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="124">
@@ -6176,7 +7284,7 @@
         <v>0.99936743272283901</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>1232</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="125">
@@ -6193,7 +7301,7 @@
         <v>0.99887341870124957</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>1233</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="126">
@@ -6210,7 +7318,7 @@
         <v>0.99892884000347815</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>1233</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="127">
@@ -6227,7 +7335,7 @@
         <v>0.99899477224233646</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>1234</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="128">
@@ -6244,7 +7352,7 @@
         <v>0.99904541584609707</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>1234</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="129">
@@ -6261,7 +7369,7 @@
         <v>0.9994085209296637</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>1235</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="130">
@@ -6278,7 +7386,7 @@
         <v>0.99879506444637467</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>1235</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="131">
@@ -6295,7 +7403,7 @@
         <v>0.99861733406336561</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>1236</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="132">
@@ -6310,7 +7418,7 @@
         <v>1</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>1237</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="133">
@@ -6327,7 +7435,7 @@
         <v>0.99987195768105819</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>1238</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="134">
@@ -6342,7 +7450,7 @@
         <v>1</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>1238</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="135">
@@ -6359,7 +7467,7 @@
         <v>0.99886386330431354</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>1239</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="136">
@@ -6376,7 +7484,7 @@
         <v>0.99878359797005145</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>1240</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="137">
@@ -6391,7 +7499,7 @@
         <v>1</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="138">
@@ -6408,7 +7516,7 @@
         <v>0.998555223983282</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="139">
@@ -6425,7 +7533,7 @@
         <v>0.99833544985375466</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="140">
@@ -6440,7 +7548,7 @@
         <v>1</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="141">
@@ -6455,7 +7563,7 @@
         <v>1</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="142">
@@ -6470,7 +7578,7 @@
         <v>1</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>1241</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="143">
@@ -6485,7 +7593,7 @@
         <v>1</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>1242</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="144">
@@ -6500,7 +7608,7 @@
         <v>1</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>1243</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="145">
@@ -6515,7 +7623,7 @@
         <v>1</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>1244</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="146">
@@ -6532,7 +7640,7 @@
         <v>0.99842813720403356</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>1245</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="147">
@@ -6549,7 +7657,7 @@
         <v>0.99909892606893824</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>1246</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="148">
@@ -6566,7 +7674,7 @@
         <v>0.99886768546308791</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>1247</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="149">
@@ -6583,7 +7691,7 @@
         <v>0.99880557538300407</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>1248</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="150">
@@ -6600,7 +7708,7 @@
         <v>0.99944005373955225</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>1248</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="151">
@@ -6617,7 +7725,7 @@
         <v>0.99975729291782645</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>1249</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="152">
@@ -6634,7 +7742,7 @@
         <v>0.99827238423397724</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>1250</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="153">
@@ -6651,7 +7759,7 @@
         <v>0.99879984214484263</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>1251</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="154">
@@ -6666,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>1252</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="155">
@@ -6683,7 +7791,7 @@
         <v>0.99902152735375704</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>1253</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="156">
@@ -6700,7 +7808,7 @@
         <v>0.99870524371517644</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>1254</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="157">
@@ -6715,7 +7823,7 @@
         <v>1</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>1254</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="158">
@@ -6732,7 +7840,7 @@
         <v>0.99878742012882582</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>1255</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="159">
@@ -6749,7 +7857,7 @@
         <v>0.99885765229630519</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>1256</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="160">
@@ -6766,7 +7874,7 @@
         <v>0.99904732692548404</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>1256</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="161">
@@ -6783,7 +7891,7 @@
         <v>0.99841523741816984</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>1257</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="162">
@@ -6800,7 +7908,7 @@
         <v>0.99942954280292284</v>
       </c>
       <c r="E162" s="0" t="s">
-        <v>1258</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="163">
@@ -6817,7 +7925,7 @@
         <v>0.99891068474929978</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>1259</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="164">
@@ -6834,7 +7942,7 @@
         <v>0.99858293463439618</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>1260</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="165">
@@ -6851,7 +7959,7 @@
         <v>0.99865651119080301</v>
       </c>
       <c r="E165" s="0" t="s">
-        <v>1260</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="166">
@@ -6868,7 +7976,7 @@
         <v>0.99969136067896824</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>1261</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="167">
@@ -6885,7 +7993,7 @@
         <v>0.99969613837743621</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>1262</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="168">
@@ -6900,7 +8008,7 @@
         <v>1</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>1263</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="169">
@@ -6915,7 +8023,7 @@
         <v>1</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>1264</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="170">
@@ -6932,7 +8040,7 @@
         <v>0.99924130148328438</v>
       </c>
       <c r="E170" s="0" t="s">
-        <v>1265</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="171">
@@ -6949,7 +8057,7 @@
         <v>0.99927092321378574</v>
       </c>
       <c r="E171" s="0" t="s">
-        <v>1266</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="172">
@@ -6966,7 +8074,7 @@
         <v>0.99859249003133221</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>1266</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="173">
@@ -6983,7 +8091,7 @@
         <v>0.99883137495473129</v>
       </c>
       <c r="E173" s="0" t="s">
-        <v>1267</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="174">
@@ -7000,7 +8108,7 @@
         <v>0.99876735379526016</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>1267</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="175">
@@ -7017,7 +8125,7 @@
         <v>0.99873582098537161</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>1268</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="176">
@@ -7034,7 +8142,7 @@
         <v>0.99908363743384088</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>1268</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="177">
@@ -7051,7 +8159,7 @@
         <v>0.99936265502437105</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>1268</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="178">
@@ -7068,7 +8176,7 @@
         <v>0.99923079054665476</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>1269</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="179">
@@ -7085,7 +8193,7 @@
         <v>0.9993550107068222</v>
       </c>
       <c r="E179" s="0" t="s">
-        <v>1270</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="180">
@@ -7102,7 +8210,7 @@
         <v>0.99863644485723768</v>
       </c>
       <c r="E180" s="0" t="s">
-        <v>1270</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="181">
@@ -7119,7 +8227,7 @@
         <v>0.99826378437673502</v>
       </c>
       <c r="E181" s="0" t="s">
-        <v>1271</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="182">
@@ -7136,7 +8244,7 @@
         <v>0.99935883286559657</v>
       </c>
       <c r="E182" s="0" t="s">
-        <v>1271</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="183">
@@ -7153,7 +8261,7 @@
         <v>0.99916294722840937</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>1272</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="184">
@@ -7168,7 +8276,7 @@
         <v>1</v>
       </c>
       <c r="E184" s="0" t="s">
-        <v>1273</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="185">
@@ -7185,7 +8293,7 @@
         <v>0.99845584785514796</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>1274</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="186">
@@ -7202,7 +8310,7 @@
         <v>0.9994744531685219</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>1274</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="187">
@@ -7219,7 +8327,7 @@
         <v>0.99924703472144571</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>1275</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="188">
@@ -7236,7 +8344,7 @@
         <v>0.99951649691504008</v>
       </c>
       <c r="E188" s="0" t="s">
-        <v>1276</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="189">
@@ -7253,7 +8361,7 @@
         <v>0.99947158654944113</v>
       </c>
       <c r="E189" s="0" t="s">
-        <v>1277</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="190">
@@ -7268,7 +8376,7 @@
         <v>1</v>
       </c>
       <c r="E190" s="0" t="s">
-        <v>1278</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="191">
@@ -7283,7 +8391,7 @@
         <v>1</v>
       </c>
       <c r="E191" s="0" t="s">
-        <v>1279</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="192">
@@ -7300,7 +8408,7 @@
         <v>0.9989068625905253</v>
       </c>
       <c r="E192" s="0" t="s">
-        <v>1280</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="193">
@@ -7317,7 +8425,7 @@
         <v>0.99908172635445369</v>
       </c>
       <c r="E193" s="0" t="s">
-        <v>1281</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="194">
@@ -7334,7 +8442,7 @@
         <v>0.99852560225278042</v>
       </c>
       <c r="E194" s="0" t="s">
-        <v>1281</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="195">
@@ -7351,7 +8459,7 @@
         <v>0.99903777152854822</v>
       </c>
       <c r="E195" s="0" t="s">
-        <v>1282</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="196">
@@ -7368,7 +8476,7 @@
         <v>0.99948687518453871</v>
       </c>
       <c r="E196" s="0" t="s">
-        <v>1283</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="197">
@@ -7385,7 +8493,7 @@
         <v>0.99965696124999881</v>
       </c>
       <c r="E197" s="0" t="s">
-        <v>1284</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="198">
@@ -7402,7 +8510,7 @@
         <v>0.99872913220751647</v>
       </c>
       <c r="E198" s="0" t="s">
-        <v>1285</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="199">
@@ -7419,7 +8527,7 @@
         <v>0.99906930433843688</v>
       </c>
       <c r="E199" s="0" t="s">
-        <v>1286</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="200">
@@ -7436,7 +8544,7 @@
         <v>0.99909128175138973</v>
       </c>
       <c r="E200" s="0" t="s">
-        <v>1286</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="201">
@@ -7453,7 +8561,7 @@
         <v>0.99912950333913353</v>
       </c>
       <c r="E201" s="0" t="s">
-        <v>1287</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="202">
@@ -7470,7 +8578,7 @@
         <v>0.99864504471448001</v>
       </c>
       <c r="E202" s="0" t="s">
-        <v>1287</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="203">
@@ -7487,7 +8595,7 @@
         <v>0.99862115622213998</v>
       </c>
       <c r="E203" s="0" t="s">
-        <v>1288</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="204">
@@ -7502,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="E204" s="0" t="s">
-        <v>1288</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="205">
@@ -7517,7 +8625,7 @@
         <v>1</v>
       </c>
       <c r="E205" s="0" t="s">
-        <v>1289</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="206">
@@ -7532,7 +8640,7 @@
         <v>1</v>
       </c>
       <c r="E206" s="0" t="s">
-        <v>1290</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="207">
@@ -7547,7 +8655,7 @@
         <v>1</v>
       </c>
       <c r="E207" s="0" t="s">
-        <v>1291</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="208">
@@ -7564,7 +8672,7 @@
         <v>0.99933494437325687</v>
       </c>
       <c r="E208" s="0" t="s">
-        <v>1292</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="209">
@@ -7581,7 +8689,7 @@
         <v>0.99941425416782526</v>
       </c>
       <c r="E209" s="0" t="s">
-        <v>1293</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="210">
@@ -7598,7 +8706,7 @@
         <v>0.99956522943941351</v>
       </c>
       <c r="E210" s="0" t="s">
-        <v>1294</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="211">
@@ -7615,7 +8723,7 @@
         <v>0.99945247575556906</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>1295</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="212">
@@ -7632,7 +8740,7 @@
         <v>0.99929385616643196</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>1296</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="213">
@@ -7649,7 +8757,7 @@
         <v>0.99906930433843677</v>
       </c>
       <c r="E213" s="0" t="s">
-        <v>1297</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="214">
@@ -7664,7 +8772,7 @@
         <v>1</v>
       </c>
       <c r="E214" s="0" t="s">
-        <v>1298</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="215">
@@ -7681,7 +8789,7 @@
         <v>0.99965313909122444</v>
       </c>
       <c r="E215" s="0" t="s">
-        <v>1299</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="216">
@@ -7698,7 +8806,7 @@
         <v>0.99855044628481393</v>
       </c>
       <c r="E216" s="0" t="s">
-        <v>1300</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="217">
@@ -7715,7 +8823,7 @@
         <v>0.99806407658077334</v>
       </c>
       <c r="E217" s="0" t="s">
-        <v>1301</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="218">
@@ -7732,7 +8840,7 @@
         <v>0.99908459297353458</v>
       </c>
       <c r="E218" s="0" t="s">
-        <v>1302</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="219">
@@ -7749,7 +8857,7 @@
         <v>0.99857815693592811</v>
       </c>
       <c r="E219" s="0" t="s">
-        <v>1303</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="220">
@@ -7766,7 +8874,7 @@
         <v>0.9986870884609983</v>
       </c>
       <c r="E220" s="0" t="s">
-        <v>1304</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="221">
@@ -7783,7 +8891,7 @@
         <v>0.99898235022631954</v>
       </c>
       <c r="E221" s="0" t="s">
-        <v>1305</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="222">
@@ -7800,7 +8908,7 @@
         <v>0.99930341156336799</v>
       </c>
       <c r="E222" s="0" t="s">
-        <v>1305</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="223">
@@ -7817,7 +8925,7 @@
         <v>0.9990425492270163</v>
       </c>
       <c r="E223" s="0" t="s">
-        <v>1306</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="224">
@@ -7834,7 +8942,7 @@
         <v>0.99945247575556906</v>
       </c>
       <c r="E224" s="0" t="s">
-        <v>1306</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="225">
@@ -7851,7 +8959,7 @@
         <v>0.99953274108983126</v>
       </c>
       <c r="E225" s="0" t="s">
-        <v>1307</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="226">
@@ -7868,7 +8976,7 @@
         <v>0.99927952307102819</v>
       </c>
       <c r="E226" s="0" t="s">
-        <v>1307</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="227">
@@ -7885,7 +8993,7 @@
         <v>0.99935309962743513</v>
       </c>
       <c r="E227" s="0" t="s">
-        <v>1307</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="228">
@@ -7902,7 +9010,7 @@
         <v>0.99916199168871578</v>
       </c>
       <c r="E228" s="0" t="s">
-        <v>1308</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="229">
@@ -7919,7 +9027,7 @@
         <v>0.99937125488161338</v>
       </c>
       <c r="E229" s="0" t="s">
-        <v>1308</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="230">
@@ -7936,7 +9044,7 @@
         <v>0.99853515764971634</v>
       </c>
       <c r="E230" s="0" t="s">
-        <v>1309</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="231">
@@ -7953,7 +9061,7 @@
         <v>0.99891832906684852</v>
       </c>
       <c r="E231" s="0" t="s">
-        <v>1309</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="232">
@@ -7968,7 +9076,7 @@
         <v>1</v>
       </c>
       <c r="E232" s="0" t="s">
-        <v>1309</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="233">
@@ -7983,7 +9091,7 @@
         <v>1</v>
       </c>
       <c r="E233" s="0" t="s">
-        <v>1309</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="234">
@@ -8000,7 +9108,7 @@
         <v>0.99962351736072297</v>
       </c>
       <c r="E234" s="0" t="s">
-        <v>1310</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="235">
@@ -8017,7 +9125,7 @@
         <v>0.99949356396239375</v>
       </c>
       <c r="E235" s="0" t="s">
-        <v>1310</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="236">
@@ -8034,7 +9142,7 @@
         <v>0.99909892606893824</v>
       </c>
       <c r="E236" s="0" t="s">
-        <v>1310</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="237">
@@ -8051,7 +9159,7 @@
         <v>0.99845775893453514</v>
       </c>
       <c r="E237" s="0" t="s">
-        <v>1311</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="238">
@@ -8066,7 +9174,7 @@
         <v>1</v>
       </c>
       <c r="E238" s="0" t="s">
-        <v>1312</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="239">
@@ -8081,7 +9189,7 @@
         <v>1</v>
       </c>
       <c r="E239" s="0" t="s">
-        <v>1313</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="240">
@@ -8098,7 +9206,7 @@
         <v>0.99774779294219273</v>
       </c>
       <c r="E240" s="0" t="s">
-        <v>1314</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="241">
@@ -8115,7 +9223,7 @@
         <v>0.99847686972840688</v>
       </c>
       <c r="E241" s="0" t="s">
-        <v>1314</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="242">
@@ -8132,7 +9240,7 @@
         <v>0.99950694151810404</v>
       </c>
       <c r="E242" s="0" t="s">
-        <v>1315</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="243">
@@ -8149,7 +9257,7 @@
         <v>0.99921359083216987</v>
       </c>
       <c r="E243" s="0" t="s">
-        <v>1316</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="244">
@@ -8166,7 +9274,7 @@
         <v>0.9984109374895489</v>
       </c>
       <c r="E244" s="0" t="s">
-        <v>1317</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="245">
@@ -8183,7 +9291,7 @@
         <v>0.99883615265319936</v>
       </c>
       <c r="E245" s="0" t="s">
-        <v>1317</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="246">
@@ -8200,7 +9308,7 @@
         <v>0.99920594651462114</v>
       </c>
       <c r="E246" s="0" t="s">
-        <v>1317</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="247">
@@ -8217,7 +9325,7 @@
         <v>0.99920594651462114</v>
       </c>
       <c r="E247" s="0" t="s">
-        <v>1318</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="248">
@@ -8234,7 +9342,7 @@
         <v>0.99883519711350577</v>
       </c>
       <c r="E248" s="0" t="s">
-        <v>1319</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="249">
@@ -8251,7 +9359,7 @@
         <v>0.99865460011141605</v>
       </c>
       <c r="E249" s="0" t="s">
-        <v>1320</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="250">
@@ -8268,7 +9376,7 @@
         <v>0.99930914480152966</v>
       </c>
       <c r="E250" s="0" t="s">
-        <v>1320</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="251">
@@ -8285,7 +9393,7 @@
         <v>0.99942285402506759</v>
       </c>
       <c r="E251" s="0" t="s">
-        <v>1321</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="252">
@@ -8300,7 +9408,7 @@
         <v>1</v>
       </c>
       <c r="E252" s="0" t="s">
-        <v>1322</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="253">
@@ -8315,7 +9423,7 @@
         <v>1</v>
       </c>
       <c r="E253" s="0" t="s">
-        <v>1323</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="254">
@@ -8332,7 +9440,7 @@
         <v>0.99796183383355841</v>
       </c>
       <c r="E254" s="0" t="s">
-        <v>1323</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="255">
@@ -8349,7 +9457,7 @@
         <v>0.99878646458913223</v>
       </c>
       <c r="E255" s="0" t="s">
-        <v>1324</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="256">
@@ -8364,7 +9472,7 @@
         <v>1</v>
       </c>
       <c r="E256" s="0" t="s">
-        <v>1325</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="257">
@@ -8379,7 +9487,7 @@
         <v>1</v>
       </c>
       <c r="E257" s="0" t="s">
-        <v>1325</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="258">
@@ -8396,7 +9504,7 @@
         <v>0.99887532978063676</v>
       </c>
       <c r="E258" s="0" t="s">
-        <v>1326</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="259">
@@ -8413,7 +9521,7 @@
         <v>0.9987625760967922</v>
       </c>
       <c r="E259" s="0" t="s">
-        <v>1326</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="260">
@@ -8430,7 +9538,7 @@
         <v>0.99873486544567802</v>
       </c>
       <c r="E260" s="0" t="s">
-        <v>1327</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="261">
@@ -8447,7 +9555,7 @@
         <v>0.99870811033425722</v>
       </c>
       <c r="E261" s="0" t="s">
-        <v>1328</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="262">
@@ -8464,7 +9572,7 @@
         <v>0.99937889919916223</v>
       </c>
       <c r="E262" s="0" t="s">
-        <v>1329</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="263">
@@ -8481,7 +9589,7 @@
         <v>0.99931105588091684</v>
       </c>
       <c r="E263" s="0" t="s">
-        <v>1329</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="264">
@@ -8496,7 +9604,7 @@
         <v>1</v>
       </c>
       <c r="E264" s="0" t="s">
-        <v>1330</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="265">
@@ -8511,7 +9619,7 @@
         <v>1</v>
       </c>
       <c r="E265" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="266">
@@ -8528,7 +9636,7 @@
         <v>0.99927283429317293</v>
       </c>
       <c r="E266" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="267">
@@ -8545,7 +9653,7 @@
         <v>0.99927283429317293</v>
       </c>
       <c r="E267" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="268">
@@ -8562,7 +9670,7 @@
         <v>0.99903586044916104</v>
       </c>
       <c r="E268" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="269">
@@ -8579,7 +9687,7 @@
         <v>0.99887962970925792</v>
       </c>
       <c r="E269" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="270">
@@ -8596,7 +9704,7 @@
         <v>0.99876830933495397</v>
       </c>
       <c r="E270" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="271">
@@ -8613,7 +9721,7 @@
         <v>0.99854614635619277</v>
       </c>
       <c r="E271" s="0" t="s">
-        <v>1331</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="272">
@@ -8630,7 +9738,7 @@
         <v>0.99937985473885582</v>
       </c>
       <c r="E272" s="0" t="s">
-        <v>1332</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="273">
@@ -8645,7 +9753,7 @@
         <v>1</v>
       </c>
       <c r="E273" s="0" t="s">
-        <v>1332</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="274">
@@ -8660,7 +9768,7 @@
         <v>1</v>
       </c>
       <c r="E274" s="0" t="s">
-        <v>1333</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="275">
@@ -8677,7 +9785,7 @@
         <v>0.99983182501392698</v>
       </c>
       <c r="E275" s="0" t="s">
-        <v>1334</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="276">
@@ -8694,7 +9802,7 @@
         <v>0.99933303329386969</v>
       </c>
       <c r="E276" s="0" t="s">
-        <v>1335</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="277">
@@ -8711,7 +9819,7 @@
         <v>0.99914479197423112</v>
       </c>
       <c r="E277" s="0" t="s">
-        <v>1335</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="278">
@@ -8728,7 +9836,7 @@
         <v>0.99898999454386839</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>1336</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="279">
@@ -8745,7 +9853,7 @@
         <v>0.99931487803969121</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>1336</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="280">
@@ -8762,7 +9870,7 @@
         <v>0.99873486544567813</v>
       </c>
       <c r="E280" s="0" t="s">
-        <v>1337</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="281">
@@ -8779,7 +9887,7 @@
         <v>0.99799718880222144</v>
       </c>
       <c r="E281" s="0" t="s">
-        <v>1337</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="282">
@@ -8796,7 +9904,7 @@
         <v>0.99886099668523276</v>
       </c>
       <c r="E282" s="0" t="s">
-        <v>1338</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="283">
@@ -8813,7 +9921,7 @@
         <v>0.99920307989554036</v>
       </c>
       <c r="E283" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="284">
@@ -8830,7 +9938,7 @@
         <v>0.99908841513230895</v>
       </c>
       <c r="E284" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="285">
@@ -8847,7 +9955,7 @@
         <v>0.99944483143802032</v>
       </c>
       <c r="E285" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="286">
@@ -8864,7 +9972,7 @@
         <v>0.9989756614484645</v>
       </c>
       <c r="E286" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="287">
@@ -8881,7 +9989,7 @@
         <v>0.99935692178620938</v>
       </c>
       <c r="E287" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="288">
@@ -8898,7 +10006,7 @@
         <v>0.99937603258008145</v>
       </c>
       <c r="E288" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="289">
@@ -8915,7 +10023,7 @@
         <v>0.99902630505222501</v>
       </c>
       <c r="E289" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="290">
@@ -8932,7 +10040,7 @@
         <v>0.99948496410515153</v>
       </c>
       <c r="E290" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="291">
@@ -8949,7 +10057,7 @@
         <v>0.99948591964484512</v>
       </c>
       <c r="E291" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="292">
@@ -8966,7 +10074,7 @@
         <v>0.99870333263578948</v>
       </c>
       <c r="E292" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="293">
@@ -8983,7 +10091,7 @@
         <v>0.99867562198467497</v>
       </c>
       <c r="E293" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="294">
@@ -8998,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="E294" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="295">
@@ -9013,7 +10121,7 @@
         <v>1</v>
       </c>
       <c r="E295" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="296">
@@ -9030,7 +10138,7 @@
         <v>0.99709038163299835</v>
       </c>
       <c r="E296" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="297">
@@ -9047,7 +10155,7 @@
         <v>0.99844438137882463</v>
       </c>
       <c r="E297" s="0" t="s">
-        <v>1339</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="298">
@@ -9062,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="E298" s="0" t="s">
-        <v>1340</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="299">
@@ -9077,7 +10185,7 @@
         <v>1</v>
       </c>
       <c r="E299" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="300">
@@ -9092,7 +10200,7 @@
         <v>1</v>
       </c>
       <c r="E300" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="301">
@@ -9107,7 +10215,7 @@
         <v>1</v>
       </c>
       <c r="E301" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="302">
@@ -9122,7 +10230,7 @@
         <v>1</v>
       </c>
       <c r="E302" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="303">
@@ -9137,7 +10245,7 @@
         <v>1</v>
       </c>
       <c r="E303" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="304">
@@ -9152,7 +10260,7 @@
         <v>1</v>
       </c>
       <c r="E304" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="305">
@@ -9167,7 +10275,7 @@
         <v>1</v>
       </c>
       <c r="E305" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="306">
@@ -9182,7 +10290,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="307">
@@ -9197,7 +10305,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="308">
@@ -9212,7 +10320,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="309">
@@ -9227,7 +10335,7 @@
         <v>1</v>
       </c>
       <c r="E309" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="310">
@@ -9242,7 +10350,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="311">
@@ -9257,7 +10365,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="312">
@@ -9274,7 +10382,7 @@
         <v>0.99903394936977374</v>
       </c>
       <c r="E312" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="313">
@@ -9291,7 +10399,7 @@
         <v>0.99897136151984312</v>
       </c>
       <c r="E313" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="314">
@@ -9306,7 +10414,7 @@
         <v>1</v>
       </c>
       <c r="E314" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="315">
@@ -9323,7 +10431,7 @@
         <v>0.99879793106545545</v>
       </c>
       <c r="E315" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="316">
@@ -9340,7 +10448,7 @@
         <v>0.99862497838091446</v>
       </c>
       <c r="E316" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="317">
@@ -9357,7 +10465,7 @@
         <v>0.99878168689066427</v>
       </c>
       <c r="E317" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="318">
@@ -9374,7 +10482,7 @@
         <v>0.99904732692548404</v>
       </c>
       <c r="E318" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="319">
@@ -9391,7 +10499,7 @@
         <v>0.99912185902158468</v>
       </c>
       <c r="E319" s="0" t="s">
-        <v>1341</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="320">
@@ -9408,7 +10516,7 @@
         <v>0.99816631932798816</v>
       </c>
       <c r="E320" s="0" t="s">
-        <v>1342</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="321">
@@ -9425,7 +10533,7 @@
         <v>0.99810038708912985</v>
       </c>
       <c r="E321" s="0" t="s">
-        <v>1343</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="322">
@@ -9442,7 +10550,7 @@
         <v>0.99851795793523146</v>
       </c>
       <c r="E322" s="0" t="s">
-        <v>1344</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="323">
@@ -9459,7 +10567,7 @@
         <v>0.99855379067374161</v>
       </c>
       <c r="E323" s="0" t="s">
-        <v>1344</v>
+        <v>1712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>